<commit_message>
updated networking correlation output ngram no len
</commit_message>
<xml_diff>
--- a/output/net comparision.xlsx
+++ b/output/net comparision.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\PycharmProjects\placement\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KRG\Desktop\github_repo_placement\placement_analysis\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53651C5-D6A8-4DF1-BA59-A0CE4B5EC5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_output_for_networking_ber" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="264">
   <si>
     <t>Text</t>
   </si>
@@ -721,12 +722,102 @@
   </si>
   <si>
     <t>['0.36', '0.29', '0.27']</t>
+  </si>
+  <si>
+    <t>['0.56', '0.52', '0.5']</t>
+  </si>
+  <si>
+    <t>['0.6', '0.39', '0.39']</t>
+  </si>
+  <si>
+    <t>['0.52', '0.41', '0.36']</t>
+  </si>
+  <si>
+    <t>['0.51', '0.37', '0.35']</t>
+  </si>
+  <si>
+    <t>['0.62', '0.5', '0.46']</t>
+  </si>
+  <si>
+    <t>['0.73', '0.55', '0.48']</t>
+  </si>
+  <si>
+    <t>['0.7', '0.5', '0.48']</t>
+  </si>
+  <si>
+    <t>['0.71', '0.45', '0.43']</t>
+  </si>
+  <si>
+    <t>['0.64', '0.46', '0.43']</t>
+  </si>
+  <si>
+    <t>['0.45', '0.39', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.32', '0.27', '0.25']</t>
+  </si>
+  <si>
+    <t>['0.44', '0.42', '0.39']</t>
+  </si>
+  <si>
+    <t>['0.57', '0.49', '0.41']</t>
+  </si>
+  <si>
+    <t>['0.4', '0.39', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.43', '0.41', '0.39']</t>
+  </si>
+  <si>
+    <t>['0.59', '0.56', '0.54']</t>
+  </si>
+  <si>
+    <t>['0.59', '0.5', '0.39']</t>
+  </si>
+  <si>
+    <t>['0.72', '0.65', '0.46']</t>
+  </si>
+  <si>
+    <t>['0.7', '0.41', '0.31']</t>
+  </si>
+  <si>
+    <t>['0.62', '0.54', '0.52']</t>
+  </si>
+  <si>
+    <t>['0.59', '0.45', '0.44']</t>
+  </si>
+  <si>
+    <t>['0.58', '0.54', '0.51']</t>
+  </si>
+  <si>
+    <t>['0.38', '0.35', '0.33']</t>
+  </si>
+  <si>
+    <t>['0.8', '0.47', '0.45']</t>
+  </si>
+  <si>
+    <t>['0.61', '0.43', '0.42']</t>
+  </si>
+  <si>
+    <t>['0.66', '0.47', '0.42']</t>
+  </si>
+  <si>
+    <t>['0.45', '0.43', '0.36']</t>
+  </si>
+  <si>
+    <t>['0.33', '0.29', '0.28']</t>
+  </si>
+  <si>
+    <t>after prepro correlation ngram no len</t>
+  </si>
+  <si>
+    <t>How does NAT (Network Address Translation) work?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1526,19 +1617,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" customWidth="1"/>
+    <col min="1" max="1" width="53.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1560,8 +1651,11 @@
       <c r="Q1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1583,8 +1677,11 @@
       <c r="Q2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1606,8 +1703,11 @@
       <c r="Q3" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1629,8 +1729,11 @@
       <c r="Q4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T4" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1652,8 +1755,11 @@
       <c r="Q5" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1675,8 +1781,11 @@
       <c r="Q6" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1698,8 +1807,11 @@
       <c r="Q7" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1721,8 +1833,11 @@
       <c r="Q8" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T8" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1744,8 +1859,11 @@
       <c r="Q9" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1767,13 +1885,13 @@
       <c r="Q10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
+        <v>263</v>
       </c>
       <c r="E11" t="s">
         <v>77</v>
@@ -1790,13 +1908,16 @@
       <c r="Q11" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T11" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
         <v>78</v>
@@ -1813,13 +1934,16 @@
       <c r="Q12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>79</v>
@@ -1836,13 +1960,16 @@
       <c r="Q13" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E14" t="s">
         <v>80</v>
@@ -1859,13 +1986,16 @@
       <c r="Q14" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T14" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E15" t="s">
         <v>81</v>
@@ -1882,13 +2012,16 @@
       <c r="Q15" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>82</v>
@@ -1905,13 +2038,16 @@
       <c r="Q16" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T16" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
         <v>83</v>
@@ -1928,13 +2064,16 @@
       <c r="Q17" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T17" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
         <v>84</v>
@@ -1951,13 +2090,16 @@
       <c r="Q18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T18" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
         <v>85</v>
@@ -1974,13 +2116,16 @@
       <c r="Q19" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T19" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
         <v>86</v>
@@ -1997,13 +2142,16 @@
       <c r="Q20" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T20" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E21" t="s">
         <v>87</v>
@@ -2020,13 +2168,16 @@
       <c r="Q21" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
         <v>88</v>
@@ -2043,13 +2194,16 @@
       <c r="Q22" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T22" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E23" t="s">
         <v>89</v>
@@ -2066,13 +2220,16 @@
       <c r="Q23" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
         <v>90</v>
@@ -2089,13 +2246,16 @@
       <c r="Q24" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T24" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
         <v>91</v>
@@ -2112,13 +2272,16 @@
       <c r="Q25" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E26" t="s">
         <v>92</v>
@@ -2135,13 +2298,16 @@
       <c r="Q26" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T26" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
         <v>93</v>
@@ -2158,13 +2324,16 @@
       <c r="Q27" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T27" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28" t="s">
         <v>94</v>
@@ -2181,13 +2350,16 @@
       <c r="Q28" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
         <v>95</v>
@@ -2204,13 +2376,16 @@
       <c r="Q29" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T29" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30" t="s">
         <v>96</v>
@@ -2227,13 +2402,16 @@
       <c r="Q30" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T30" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E31" t="s">
         <v>97</v>
@@ -2250,13 +2428,16 @@
       <c r="Q31" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
         <v>98</v>
@@ -2273,13 +2454,16 @@
       <c r="Q32" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T32" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E33" t="s">
         <v>99</v>
@@ -2296,13 +2480,16 @@
       <c r="Q33" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T33" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E34" t="s">
         <v>100</v>
@@ -2319,8 +2506,17 @@
       <c r="Q34" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="T34" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
       <c r="E35" t="s">
         <v>101</v>
       </c>
@@ -2335,6 +2531,9 @@
       </c>
       <c r="Q35" t="s">
         <v>201</v>
+      </c>
+      <c r="T35" t="s">
+        <v>261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>